<commit_message>
Label Powerset Results: MNB and SVM
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
+++ b/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="127">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -48,388 +48,361 @@
     <t xml:space="preserve">Count Vectorizer</t>
   </si>
   <si>
-    <t xml:space="preserve">0.163 0.768 0.612 0.202 0.651</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.575 0.629 0.693 0.640 0.926</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.089 0.767 0.453 0.113 0.483</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.897 0.768 0.834 0.890 0.953</t>
+    <t xml:space="preserve">0.421 0.747 0.700 0.379 0.742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.378 0.590 0.582 0.453 0.693</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.270 0.769 0.580 0.236 0.599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.876 0.741 0.814 0.878 0.944</t>
   </si>
   <si>
     <t xml:space="preserve">Support Vector Machines</t>
   </si>
   <si>
-    <t xml:space="preserve">0.462 0.742 0.708 0.553 0.812</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.427 0.709 0.645 0.474 0.808</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.305 0.651 0.580 0.391 0.691</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.883 0.791 0.836 0.879 0.960</t>
+    <t xml:space="preserve">0.397 0.760 0.680 0.527 0.779</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.351 0.671 0.596 0.444 0.836</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.251 0.705 0.549 0.366 0.643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.872 0.783 0.817 0.873 0.959</t>
   </si>
   <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF</t>
   </si>
   <si>
-    <t xml:space="preserve">0.416 0.740 0.719 0.609 0.845</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.383 0.584 0.501 0.321 0.606</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.266 0.755 0.641 0.468 0.758</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.877 0.735 0.778 0.823 0.938</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.417 0.725 0.694 0.522 0.786</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.437 0.699 0.671 0.507 0.839</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.266 0.626 0.556 0.359 0.652</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.886 0.782 0.841 0.885 0.960</t>
+    <t xml:space="preserve">0.430 0.728 0.712 0.604 0.832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.379 0.592 0.508 0.290 0.626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.278 0.705 0.624 0.468 0.734</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.875 0.736 0.783 0.805 0.940</t>
   </si>
   <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(3)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.311 0.747 0.735 0.539 0.816</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.410 0.562 0.535 0.396 0.744</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.185 0.876 0.654 0.380 0.700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.886 0.727 0.797 0.861 0.954</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.426 0.728 0.671 0.500 0.709 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.418 0.705 0.698 0.511 0.905</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.274 0.628 0.523 0.338 0.551</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.883 0.785 0.844 0.886 0.957</t>
+    <t xml:space="preserve">0.366 0.736 0.708 0.595 0.778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.291 0.574 0.493 0.301 0.634</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.228 0.762 0.624 0.454 0.652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.859 0.728 0.774 0.814 0.939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.387 0.746 0.644 0.518 0.738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.366 0.667 0.557 0.402 0.797 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.243 0.679 0.506 0.359 0.589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.875 0.777 0.801 0.863 0.953</t>
   </si>
   <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(2)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.342 0.773 0.742 0.590 0.825</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.372 0.602 0.538 0.327 0.659</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.208 0.841 0.667 0.444 0.720</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.879 0.758 0.799 0.830 0.945</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.421 0.739 0.667 0.507 0.743</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.422 0.714 0.669 0.492 0.885</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.270 0.644 0.521 0.345 0.594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.883 0.792 0.836 0.883 0.959</t>
+    <t xml:space="preserve">0.367 0.740 0.715 0.583 0.790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.317 0.586 0.494 0.282 0.612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.228 0.752 0.637 0.444 0.671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.866 0.736 0.774 0.804 0.936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.416 0.748 0.663 0.522 0.774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.381 0.667 0.577 0.412 0.776</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.266 0.685 0.529 0.363 0.638</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.877 0.778 0.809 0.866 0.954</t>
   </si>
   <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1)</t>
   </si>
   <si>
+    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.420 0.719 0.688 0.514 0.842</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.359 0.609 0.491 0.257 0.561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.270 0.665 0.589 0.366 0.758</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.872 0.742 0.773 0.803 0.929</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.368 0.726 0.624 0.361 0.790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.373 0.678 0.596 0.460 0.761</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.228 0.636 0.475 0.222 0.662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.878 0.775 0.812 0.879 0.954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords + Lemm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.690 0.568 0.208 0.252 0.399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.493 0.550 0.342 0.344 0.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.606 0.407 0.116 0.145 0.250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.754 0.855 0.920 0.916 0.974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.637 0.645 0.434 0.500 0.517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.611 0.521 0.301 0.425 0.538</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.493 0.498 0.281 0.338 0.350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.801 0.849 0.901 0.917 0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.654 0.683 0.524 0.602 0.601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.487 0.373 0.214 0.240 0.224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.546 0.587 0.371 0.456 0.438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.751 0.780 0.855 0.853 0.946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.801 0.849 0.901 0.917 0.975 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.667 0.676 0.547 0.615 0.599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.468 0.352 0.204 0.233 0.192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.577 0.585 0.397 0.474 0.438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.739 0.766 0.844 0.846 0.938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.585 0.625 0.444 0.481 0.490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.563 0.499 0.297 0.410 0.520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.435 0.475 0.290 0.320 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.782 0.843 0.899 0.916 0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.656 0.670 0.535 0.621 0.599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.473 0.358 0.202 0.231 0.180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.556 0.572 0.384 0.482 0.438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.742 0.772 0.845 0.843 0.934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.587 0.613 0.444 0.495 0.489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.561 0.486 0.286 0.427 0.491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.438 0.463 0.290 0.333 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.781 0.839 0.896 0.918 0.974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.602 0.666 0.513 0.568 0.610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.461 0.363 0.196 0.233 0.185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.475 0.562 0.362 0.417 0.450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.738 0.777 0.846 0.855 0.934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.583 0.572 0.369 0.420 0.504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.555 0.521 0.425 0.484 0.794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.434 0.413 0.228 0.268 0.338</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.779 0.848 0.922 0.925 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.771 0.505 0.182 0.222 0.692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.546 0.557 0.380 0.475 0.873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.748 0.344 0.101 0.125 0.530 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.784 0.863 0.928 0.945 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.693 0.653 0.435 0.507 0.821</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.635 0.555 0.366 0.448 0.774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.566 0.502 0.280 0.342 0.701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.812 0.867 0.918 0.941 0.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.723 0.706 0.538 0.552 0.733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.563 0.384 0.250 0.222 0.773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.636 0.615 0.381 0.395 0.581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.788 0.798 0.880 0.891 0.975 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.723 0.720 0.526 0.606 0.733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.533 0.363 0.230 0.226 0.764</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.651 0.654 0.370 0.454 0.581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.773 0.780 0.873 0.885 0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.658 0.651 0.428 0.484 0.797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.623 0.514 0.377 0.408 0.736</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.520 0.505 0.275 0.322 0.667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.804 0.857 0.920 0.937 0.976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.720 0.711 0.557 0.629 0.732</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.543 0.360 0.240 0.237 0.723</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.640 0.637 0.402 0.480 0.581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.778 0.780 0.873 0.887 0.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.687 0.670 0.402 0.528 0.809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.628 0.531 0.364 0.491 0.777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.559 0.527 0.254 0.362 0.684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.809 0.862 0.919 0.945 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.788 0.798 0.880 0.891 0.975</t>
+  </si>
+  <si>
     <t xml:space="preserve">CV + TFIDF + ngram(3) + stopwords</t>
   </si>
   <si>
-    <t xml:space="preserve">0.388 0.768 0.729 0.578 0.815</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.423 0.592 0.547 0.356 0.646</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.243 0.854 0.639 0.426 0.705</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.885 0.751 0.803 0.844 0.942</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.374 0.736 0.613 0.420 0.717</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.429 0.744 0.690 0.547 0.928</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.232 0.628 0.455 0.268 0.560</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.886 0.801 0.834 0.889 0.959</t>
+    <t xml:space="preserve">0.656 0.676 0.556 0.432 0.724</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.550 0.367 0.226 0.163 0.593</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.531 0.571 0.402 0.283 0.573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.777 0.792 0.866 0.882 0.965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.682 0.601 0.348 0.320 0.780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.660 0.566 0.455 0.453 0.862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.546 0.441 0.212 0.191 0.641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.818 0.868 0.929 0.943 0.981</t>
   </si>
   <si>
     <t xml:space="preserve">CV + TFIDF + ngram(3) + stopwords + Lemm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.423 0.592 0.547 0.356 0.646 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.543 0.469 0.085 0.198 0.222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.654 0.772 0.556 0.735 0.769</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.383 0.308 0.045 0.110 0.125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.802 0.877 0.928 0.931 0.976</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.688 0.649 0.441 0.526 0.490</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.625 0.602 0.413 0.547 0.743</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.560 0.496 0.286 0.360 0.325</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.812 0.869 0.919 0.931 0.980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.669 0.681 0.512 0.550 0.592</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.491 0.479 0.292 0.309 0.293</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.569 0.552 0.353 0.390 0.425</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.753 0.836 0.891 0.890 0.959</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.642 0.613 0.415 0.483 0.490</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.614 0.587 0.476 0.566 0.788</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.499 0.455 0.263 0.320 0.325</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.803 0.864 0.925 0.932 0.980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.698 0.622 0.332 0.481 0.570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.481 0.466 0.300 0.417 0.582</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.631 0.475 0.201 0.320 0.400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.746 0.832 0.908 0.917 0.977</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.622 0.598 0.409 0.425 0.447</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.588 0.555 0.397 0.463 0.958</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.477 0.440 0.259 0.272 0.288</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.793 0.857 0.918 0.923 0.981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.696 0.665 0.434 0.531 0.556</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.478 0.461 0.325 0.368 0.437</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.628 0.533 0.281 0.368 0.388</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.744 0.829 0.905 0.907 0.971</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.627 0.602 0.404 0.436 0.431</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.590 0.553 0.500 0.448 0.917</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.483 0.444 0.254 0.281 0.275</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.794 0.856 0.927 0.921 0.981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.662 0.621 0.367 0.508 0.582</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.483 0.471 0.263 0.359 0.452</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.560 0.473 0.228 0.346 0.413</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.749 0.834 0.898 0.906 0.972</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.582 0.538 0.333 0.409 0.447</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.595 0.550 0.433 0.465 0.920</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.428 0.376 0.201 0.259 0.288</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.791 0.854 0.923 0.923 0.981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.674 0.453 0.138 0.180 0.670</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.672 0.676 0.538 0.682 0.922</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.534 0.295 0.074 0.099 0.504</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.821 0.875 0.933 0.948 0.977</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.740 0.666 0.429 0.447 0.798</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.688 0.652 0.441 0.449 0.813</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.624 0.512 0.275 0.289 0.667</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.837 0.888 0.927 0.942 0.980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.749 0.712 0.556 0.534 0.784</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.540 0.477 0.288 0.228 0.724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.700 0.595 0.397 0.375 0.650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.779 0.844 0.893 0.896 0.975</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.689 0.621 0.397 0.407 0.792</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.643 0.667 0.540 0.470 0.846</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.559 0.459 0.249 0.257 0.658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.815 0.886 0.935 0.944 0.981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.750 0.676 0.427 0.406 0.685</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.491 0.456 0.280 0.394 0.884</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.755 0.546 0.275 0.257 0.521</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.747 0.837 0.903 0.938 0.977</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.679 0.621 0.326 0.311 0.808</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.629 0.618 0.430 0.622 0.721</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.547 0.461 0.196 0.184 0.684</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.808 0.879 0.928 0.949 0.976</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.766 0.687 0.382 0.430 0.774</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.506 0.446 0.352 0.344 0.860</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.783 0.563 0.238 0.276 0.632</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.758 0.832 0.918 0.932 0.980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.679 0.608 0.234 0.320 0.798</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.637 0.618 0.758 0.879 0.804</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.546 0.446 0.132 0.191 0.667</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.811 0.878 0.938 0.954 0.979</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.744 0.719 0.396 0.430 0.691</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.467 0.460 0.388 0.353 0.756</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.786 0.610 0.249 0.276 0.530</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.726 0.837 0.922 0.933 0.973</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.652 0.546 0.217 0.282 0.760</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.647 0.664 0.920 0.893 0.837 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.508 0.380 0.122 0.164 0.615</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.810 0.880 0.940 0.953 0.979</t>
   </si>
 </sst>
 </file>
@@ -532,19 +505,19 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,16 +612,16 @@
         <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,19 +633,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,19 +653,19 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,19 +673,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -720,19 +693,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,15 +713,15 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="0" t="s">
@@ -760,19 +733,19 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -780,19 +753,19 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,19 +773,19 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,19 +793,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,19 +813,19 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -874,18 +847,18 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="1" sqref="C21:F22 C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,17 +888,17 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>56</v>
+      <c r="C3" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,16 +909,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -960,16 +933,16 @@
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,16 +953,16 @@
         <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,19 +974,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,19 +994,19 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,19 +1019,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,19 +1039,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,19 +1059,19 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>66</v>
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,19 +1079,19 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>57</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,19 +1099,19 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,19 +1119,19 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,19 +1139,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,19 +1159,19 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1219,19 +1192,19 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,16 +1235,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1282,16 +1255,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1309,16 +1282,16 @@
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,16 +1302,16 @@
         <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,19 +1323,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,19 +1343,19 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1395,19 +1368,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,19 +1388,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,19 +1408,19 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,19 +1428,19 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1475,19 +1448,19 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,19 +1468,19 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1515,19 +1488,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,19 +1508,19 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report: Updated Methodology section
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
+++ b/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="162">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -291,6 +291,18 @@
     <t xml:space="preserve">Logistic Regression</t>
   </si>
   <si>
+    <t xml:space="preserve">0.682 0.568 0.409 0.415 0.766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.619 0.534 0.398 0.412 0.745</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.553 0.407 0.259 0.263 0.624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.806 0.860 0.923 0.939 0.975</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.771 0.505 0.182 0.222 0.692</t>
   </si>
   <si>
@@ -318,9 +330,45 @@
     <t xml:space="preserve">Decision Tree</t>
   </si>
   <si>
+    <t xml:space="preserve">0.533 0.217 0.138 0.100 0.706</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.440 0.476 0.350 0.400 0.877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.392 0.122 0.074 0.053 0.547</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.727 0.851 0.928 0.944 0.978</t>
+  </si>
+  <si>
     <t xml:space="preserve">Random Forest</t>
   </si>
   <si>
+    <t xml:space="preserve">0.656 0.333 0.191 0.273 0.768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.648 0.943 0.952 0.828 0.913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.514 0.200 0.106 0.158 0.624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.811 0.880 0.939 0.952 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.692 0.548 0.410 0.431 0.772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.620 0.549 0.434 0.494 0.763</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.568 0.385 0.259 0.276 0.632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.807 0.863 0.927 0.945 0.976</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.723 0.706 0.538 0.552 0.733</t>
   </si>
   <si>
@@ -333,6 +381,30 @@
     <t xml:space="preserve">0.788 0.798 0.880 0.891 0.975 </t>
   </si>
   <si>
+    <t xml:space="preserve">0.662 0.340 0.200 0.292 0.768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.664 0.933 1.000 0.839 0.913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.520 0.205 0.111 0.171 0.624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.816 0.881 0.940 0.953 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.671 0.508 0.376 0.382 0.772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.597 0.566 0.389 0.434 0.755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.543 0.346 0.233 0.237 0.632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.797 0.864 0.923 0.941 0.976</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.723 0.720 0.526 0.606 0.733</t>
   </si>
   <si>
@@ -355,6 +427,30 @@
   </si>
   <si>
     <t xml:space="preserve">0.804 0.857 0.920 0.937 0.976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.562 0.201 0.156 0.100 0.692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.448 0.495 0.372 0.308 0.886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.425 0.112 0.085 0.053 0.530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.729 0.852 0.928 0.942 0.977 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.690 0.340 0.191 0.282 0.774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.646 0.875 0.952 0.806 0.937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.559 0.205 0.106 0.164 0.632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.816 0.879 0.939 0.952 0.983</t>
   </si>
   <si>
     <t xml:space="preserve">0.720 0.711 0.557 0.629 0.732</t>
@@ -520,13 +616,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -861,13 +957,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,18 +1298,18 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.3163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,6 +1346,18 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -1259,16 +1367,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1279,32 +1387,56 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,9 +1450,18 @@
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -1330,16 +1471,16 @@
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,32 +1491,56 @@
         <v>17</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C12" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1389,6 +1554,18 @@
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C15" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -1398,16 +1575,16 @@
         <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1418,32 +1595,56 @@
         <v>22</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C18" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1469,16 +1670,16 @@
         <v>31</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1489,21 +1690,21 @@
         <v>31</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>31</v>
@@ -1511,7 +1712,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>31</v>
@@ -1537,16 +1738,16 @@
         <v>40</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1557,21 +1758,21 @@
         <v>40</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>40</v>
@@ -1582,7 +1783,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>40</v>
@@ -1603,7 +1804,7 @@
         <v>88</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,19 +1812,19 @@
         <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,35 +1832,35 @@
         <v>12</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,7 +1872,7 @@
         <v>88</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,19 +1880,19 @@
         <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,35 +1900,35 @@
         <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated format for tables for fine-grained classification
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
+++ b/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="280">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -42,12 +42,15 @@
     <t xml:space="preserve">Accuracy</t>
   </si>
   <si>
+    <t xml:space="preserve">Logistic Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Vectorizer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Multinomial Naive Bayes</t>
   </si>
   <si>
-    <t xml:space="preserve">Count Vectorizer</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.421 0.747 0.700 0.379 0.742</t>
   </si>
   <si>
@@ -75,6 +78,12 @@
     <t xml:space="preserve">0.872 0.783 0.817 0.873 0.959</t>
   </si>
   <si>
+    <t xml:space="preserve">Decision Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random Forest</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF</t>
   </si>
   <si>
@@ -93,6 +102,18 @@
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(3)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.430 0.736 0.648 0.437 0.791</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.371 0.657 0.589 0.375 0.774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.278 0.667 0.506 0.285 0.662 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.874 0.769 0.812 0.862 0.955</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.366 0.736 0.708 0.595 0.778</t>
   </si>
   <si>
@@ -117,9 +138,45 @@
     <t xml:space="preserve">0.875 0.777 0.801 0.863 0.953</t>
   </si>
   <si>
+    <t xml:space="preserve">0.350 0.656 0.360 0.224 0.688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.247 0.513 0.517 0.275 0.858 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.216 0.617 0.223 0.127 0.527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.847 0.672 0.781 0.860 0.953 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.238 0.765 0.533 0.304 0.732</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.538 0.611 0.758 0.729 0.870</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.135 0.790 0.368 0.180 0.580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.896 0.758 0.834 0.897 0.957</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(2)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.401 0.745 0.647 0.408 0.773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.342 0.662 0.603 0.357 0.759 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.255 0.680 0.503 0.261 0.638 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.869 0.774 0.816 0.860 0.952 </t>
+  </si>
+  <si>
     <t xml:space="preserve">0.367 0.740 0.715 0.583 0.790</t>
   </si>
   <si>
@@ -144,12 +201,54 @@
     <t xml:space="preserve">0.877 0.778 0.809 0.866 0.954</t>
   </si>
   <si>
+    <t xml:space="preserve">0.355 0.665 0.368 0.213 0.688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.247 0.521 0.537 0.315 0.865 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.220 0.630 0.228 0.120 0.527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.846 0.679 0.785 0.868 0.953 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.306 0.773 0.549 0.362 0.727 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.588 0.624 0.726 0.677 0.826</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.181 0.789 0.385 0.222 0.575 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.900 0.768 0.831 0.897 0.954</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.847 0.672 0.781 0.860 0.953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.238 0.765 0.533 0.304 0.732 </t>
+  </si>
+  <si>
     <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords</t>
   </si>
   <si>
+    <t xml:space="preserve">0.424 0.710 0.644 0.331 0.800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.350 0.653 0.593 0.329 0.737 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.274 0.620 0.501 0.201 0.676 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.869 0.760 0.813 0.860 0.952</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.420 0.719 0.688 0.514 0.842</t>
   </si>
   <si>
@@ -174,9 +273,45 @@
     <t xml:space="preserve">0.878 0.775 0.812 0.879 0.954</t>
   </si>
   <si>
+    <t xml:space="preserve">0.188 0.611 0.480 0.156 0.758</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.297 0.613 0.680 0.289 0.736</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.104 0.478 0.320 0.085 0.618</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.879 0.721 0.816 0.870 0.949</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.363 0.720 0.603 0.337 0.807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.367 0.688 0.679 0.430 0.759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.224 0.621 0.444 0.204 0.686 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.877 0.776 0.830 0.876 0.955</t>
+  </si>
+  <si>
     <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords + Lemm</t>
   </si>
   <si>
+    <t xml:space="preserve">0.616 0.522 0.308 0.316 0.475</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.544 0.578 0.360 0.355 0.556 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.477 0.360 0.183 0.189 0.313</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.776 0.858 0.917 0.915 0.976</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.690 0.568 0.208 0.252 0.399</t>
   </si>
   <si>
@@ -201,6 +336,42 @@
     <t xml:space="preserve">0.801 0.849 0.901 0.917 0.975</t>
   </si>
   <si>
+    <t xml:space="preserve">0.398 0.248 0.077 0.017 0.298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.403 0.442 0.333 0.105 0.583</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.257 0.143 0.040 0.009 0.175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.728 0.837 0.924 0.921 0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.467 0.308 0.229 0.292 0.491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.681 0.946 0.879 0.907 1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.309 0.182 0.129 0.171 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.798 0.870 0.936 0.937 0.983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.608 0.500 0.314 0.352 0.490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.540 0.571 0.333 0.386 0.542</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.466 0.339 0.188 0.215 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.774 0.856 0.914 0.917 0.975</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.654 0.683 0.524 0.602 0.601</t>
   </si>
   <si>
@@ -216,6 +387,30 @@
     <t xml:space="preserve">0.801 0.849 0.901 0.917 0.975 </t>
   </si>
   <si>
+    <t xml:space="preserve">0.464 0.302 0.229 0.286 0.491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.680 0.935 0.879 0.905 1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.307 0.178 0.129 0.167 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.797 0.869 0.936 0.937 0.983 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.596 0.501 0.269 0.291 0.461</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.531 0.532 0.302 0.310 0.649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.452 0.341 0.156 0.171 0.300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.771 0.850 0.913 0.911 0.978</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.667 0.676 0.547 0.615 0.599</t>
   </si>
   <si>
@@ -240,6 +435,42 @@
     <t xml:space="preserve">0.782 0.843 0.899 0.916 0.975</t>
   </si>
   <si>
+    <t xml:space="preserve">0.413 0.270 0.069 0.051 0.333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.382 0.466 0.195 0.200 0.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.272 0.157 0.036 0.026 0.200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.717 0.840 0.919 0.920 0.974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.511 0.302 0.215 0.286 0.491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.613 0.935 0.818 0.864 0.963 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.352 0.178 0.121 0.167 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.789 0.869 0.934 0.936 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.590 0.468 0.229 0.252 0.490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.524 0.558 0.269 0.306 0.667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.446 0.310 0.129 0.145 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.768 0.853 0.911 0.913 0.978</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.656 0.670 0.535 0.621 0.599</t>
   </si>
   <si>
@@ -264,6 +495,45 @@
     <t xml:space="preserve">0.781 0.839 0.896 0.918 0.974</t>
   </si>
   <si>
+    <t xml:space="preserve">0.382 0.466 0.195 0.200 0.500 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.498 0.296 0.215 0.286 0.491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.633 0.933 0.794 0.884 0.963 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.339 0.174 0.121 0.167 0.325 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.792 0.868 0.934 0.937 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.540 0.571 0.333 0.386 0.542 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.398 0.248 0.077 0.017 0.298 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.403 0.442 0.333 0.105 0.583 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.728 0.837 0.924 0.921 0.975 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.535 0.394 0.235 0.246 0.461</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.549 0.531 0.286 0.368 0.667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.380 0.248 0.134 0.140 0.300 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.774 0.848 0.913 0.919 0.978 </t>
+  </si>
+  <si>
     <t xml:space="preserve">0.602 0.666 0.513 0.568 0.610</t>
   </si>
   <si>
@@ -288,7 +558,28 @@
     <t xml:space="preserve">0.779 0.848 0.922 0.925 0.981</t>
   </si>
   <si>
-    <t xml:space="preserve">Logistic Regression</t>
+    <t xml:space="preserve">0.378 0.267 0.061 0.100 0.316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.478 0.466 0.226 0.387 0.484 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.238 0.155 0.031 0.053 0.188 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.753 0.840 0.922 0.924 0.974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.466 0.455 0.263 0.317 0.447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.559 0.649 0.486 0.652 0.920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.312 0.298 0.152 0.189 0.288 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.774 0.865 0.927 0.933 0.981</t>
   </si>
   <si>
     <t xml:space="preserve">0.682 0.568 0.409 0.415 0.766</t>
@@ -327,9 +618,6 @@
     <t xml:space="preserve">0.812 0.867 0.918 0.941 0.979</t>
   </si>
   <si>
-    <t xml:space="preserve">Decision Tree</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.533 0.217 0.138 0.100 0.706</t>
   </si>
   <si>
@@ -342,9 +630,6 @@
     <t xml:space="preserve">0.727 0.851 0.928 0.944 0.978</t>
   </si>
   <si>
-    <t xml:space="preserve">Random Forest</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.656 0.333 0.191 0.273 0.768</t>
   </si>
   <si>
@@ -453,6 +738,18 @@
     <t xml:space="preserve">0.816 0.879 0.939 0.952 0.983</t>
   </si>
   <si>
+    <t xml:space="preserve">0.702 0.542 0.355 0.431 0.791</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.621 0.592 0.366 0.433 0.778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.582 0.378 0.217 0.276 0.658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.809 0.870 0.921 0.941 0.978</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.720 0.711 0.557 0.629 0.732</t>
   </si>
   <si>
@@ -477,10 +774,46 @@
     <t xml:space="preserve">0.809 0.862 0.919 0.945 0.978</t>
   </si>
   <si>
+    <t xml:space="preserve">0.574 0.217 0.156 0.100 0.692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.452 0.510 0.400 0.296 0.886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.440 0.122 0.085 0.053 0.530 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.730 0.853 0.929 0.941 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.688 0.343 0.200 0.282 0.774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.650 0.904 0.913 0.833 0.937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.556 0.207 0.111 0.164 0.632 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.816 0.880 0.939 0.953 0.983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.807 0.863 0.927 0.945 0.976 </t>
+  </si>
+  <si>
     <t xml:space="preserve">0.788 0.798 0.880 0.891 0.975</t>
   </si>
   <si>
-    <t xml:space="preserve">CV + TFIDF + ngram(3) + stopwords</t>
+    <t xml:space="preserve">0.616 0.534 0.416 0.390 0.772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.603 0.589 0.435 0.474 0.725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.469 0.371 0.265 0.243 0.632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.793 0.869 0.927 0.944 0.974</t>
   </si>
   <si>
     <t xml:space="preserve">0.656 0.676 0.556 0.432 0.724</t>
@@ -507,7 +840,28 @@
     <t xml:space="preserve">0.818 0.868 0.929 0.943 0.981</t>
   </si>
   <si>
-    <t xml:space="preserve">CV + TFIDF + ngram(3) + stopwords + Lemm</t>
+    <t xml:space="preserve">0.447 0.269 0.119 0.123 0.699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.470 0.478 0.245 0.400 0.863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.298 0.156 0.063 0.066 0.538</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.744 0.850 0.923 0.944 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.636 0.432 0.250 0.301 0.774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.631 0.637 0.458 0.500 0.871 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.491 0.278 0.143 0.178 0.632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.803 0.870 0.930 0.945 0.981</t>
   </si>
 </sst>
 </file>
@@ -608,21 +962,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,88 +998,75 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="F5" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,203 +1074,587 @@
       <c r="B8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>29</v>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>39</v>
-      </c>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>16</v>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="E21" s="0" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="F21" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>49</v>
+      <c r="C23" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -949,21 +1673,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,88 +1709,111 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>53</v>
+        <v>92</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>57</v>
+        <v>96</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>61</v>
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,208 +1821,623 @@
       <c r="B8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>70</v>
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>79</v>
-      </c>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>127</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>62</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>63</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>82</v>
+        <v>139</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>86</v>
+        <v>143</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>87</v>
-      </c>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>82</v>
+        <v>46</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>87</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1297,19 +2458,18 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.6428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,102 +2501,102 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>89</v>
+        <v>186</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>90</v>
+        <v>187</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>91</v>
+        <v>188</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>92</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>190</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>95</v>
+        <v>192</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>97</v>
+        <v>194</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>100</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>102</v>
+        <v>198</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>103</v>
+        <v>199</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>105</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>108</v>
+        <v>203</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>110</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,102 +2605,102 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>111</v>
+        <v>206</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>112</v>
+        <v>207</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>113</v>
+        <v>208</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>114</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>115</v>
+        <v>210</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>116</v>
+        <v>211</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>117</v>
+        <v>212</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>118</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>97</v>
+        <v>194</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>100</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>102</v>
+        <v>198</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>103</v>
+        <v>199</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>105</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>119</v>
+        <v>214</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>120</v>
+        <v>215</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>121</v>
+        <v>216</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>122</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,102 +2709,102 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>123</v>
+        <v>218</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>124</v>
+        <v>219</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>125</v>
+        <v>220</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>126</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>127</v>
+        <v>222</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>128</v>
+        <v>223</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>129</v>
+        <v>224</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>131</v>
+        <v>226</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>132</v>
+        <v>227</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>133</v>
+        <v>228</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>134</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>135</v>
+        <v>230</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>136</v>
+        <v>231</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>137</v>
+        <v>232</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>138</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>139</v>
+        <v>234</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>140</v>
+        <v>235</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>141</v>
+        <v>236</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>142</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1653,69 +2813,102 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>143</v>
+        <v>242</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>144</v>
+        <v>243</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>145</v>
+        <v>244</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>146</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>147</v>
+        <v>246</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>148</v>
+        <v>247</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>149</v>
+        <v>248</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>150</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,73 +2917,103 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>67</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>115</v>
+        <v>210</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>116</v>
+        <v>211</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>117</v>
+        <v>212</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>151</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>97</v>
+        <v>194</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>100</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
@@ -1801,66 +3024,102 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>152</v>
+        <v>70</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>153</v>
+        <v>264</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>154</v>
+        <v>265</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>155</v>
+        <v>266</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>156</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>157</v>
+        <v>268</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>158</v>
+        <v>269</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>159</v>
+        <v>270</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>160</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>152</v>
+        <v>70</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>152</v>
+        <v>70</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,66 +3128,102 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>161</v>
+        <v>91</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>153</v>
+        <v>264</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>154</v>
+        <v>265</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>155</v>
+        <v>266</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>156</v>
+        <v>267</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>157</v>
+        <v>268</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>158</v>
+        <v>269</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>159</v>
+        <v>270</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>160</v>
+        <v>271</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>161</v>
+        <v>91</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>161</v>
+        <v>91</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results of Label Powerset for Config 1-5, Projects 1-3, Classifiers 1-5
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
+++ b/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="290">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -48,6 +48,18 @@
     <t xml:space="preserve">Count Vectorizer</t>
   </si>
   <si>
+    <t xml:space="preserve">0.372 0.729 0.663 0.416 0.766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.305 0.656 0.595 0.364 0.774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.232 0.652 0.525 0.268 0.628 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.863 0.767 0.815 0.861 0.953</t>
+  </si>
+  <si>
     <t xml:space="preserve">Multinomial Naive Bayes</t>
   </si>
   <si>
@@ -81,12 +93,48 @@
     <t xml:space="preserve">Decision Tree</t>
   </si>
   <si>
+    <t xml:space="preserve">0.345 0.667 0.370 0.213 0.676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.243 0.522 0.541 0.321 0.876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.212 0.635 0.230 0.120 0.512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.847 0.679 0.786 0.868 0.953</t>
+  </si>
+  <si>
     <t xml:space="preserve">Random Forest</t>
   </si>
   <si>
+    <t xml:space="preserve">0.290 0.775 0.534 0.357 0.720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.489 0.630 0.731 0.674 0.842 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.170 0.786 0.370 0.218 0.565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.893 0.771 0.830 0.897 0.954</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF</t>
   </si>
   <si>
+    <t xml:space="preserve">0.430 0.736 0.648 0.437 0.791</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.371 0.657 0.589 0.375 0.774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.216 0.617 0.223 0.127 0.527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.874 0.769 0.812 0.862 0.955</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.430 0.728 0.712 0.604 0.832</t>
   </si>
   <si>
@@ -99,21 +147,30 @@
     <t xml:space="preserve">0.875 0.736 0.783 0.805 0.940</t>
   </si>
   <si>
+    <t xml:space="preserve">0.350 0.656 0.360 0.224 0.688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.247 0.513 0.517 0.275 0.858 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.847 0.672 0.781 0.860 0.953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.238 0.765 0.533 0.304 0.732 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.538 0.611 0.758 0.729 0.870</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.135 0.790 0.368 0.180 0.580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.896 0.758 0.834 0.897 0.957</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(3)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.430 0.736 0.648 0.437 0.791</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.371 0.657 0.589 0.375 0.774</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.278 0.667 0.506 0.285 0.662 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.874 0.769 0.812 0.862 0.955</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.366 0.736 0.708 0.595 0.778</t>
   </si>
   <si>
@@ -138,28 +195,7 @@
     <t xml:space="preserve">0.875 0.777 0.801 0.863 0.953</t>
   </si>
   <si>
-    <t xml:space="preserve">0.350 0.656 0.360 0.224 0.688</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.247 0.513 0.517 0.275 0.858 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.216 0.617 0.223 0.127 0.527</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.847 0.672 0.781 0.860 0.953 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.238 0.765 0.533 0.304 0.732</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.538 0.611 0.758 0.729 0.870</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.135 0.790 0.368 0.180 0.580</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.896 0.758 0.834 0.897 0.957</t>
+    <t xml:space="preserve">0.212 0.635 0.230 0.120 0.512 </t>
   </si>
   <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(2)</t>
@@ -226,12 +262,6 @@
   </si>
   <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.847 0.672 0.781 0.860 0.953</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.238 0.765 0.533 0.304 0.732 </t>
   </si>
   <si>
     <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords</t>
@@ -965,7 +995,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1012,61 +1042,97 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,63 +1144,99 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="F11" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,99 +1248,75 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,99 +1328,99 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,99 +1432,99 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1458,99 +1536,99 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,99 +1640,99 @@
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="F41" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1724,96 +1802,96 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,99 +1903,99 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,99 +2007,99 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,99 +2111,99 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2137,99 +2215,99 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,99 +2319,99 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,99 +2423,99 @@
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2507,96 +2585,96 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2608,99 +2686,99 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2712,99 +2790,99 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,99 +2894,99 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2920,99 +2998,99 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3027,99 +3105,99 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,99 +3209,99 @@
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added keyword extraction script for IRC messages for Lucene, Thunderbird and Ubuntu
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
+++ b/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="321">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -171,6 +171,18 @@
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(3)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.367 0.736 0.659 0.445 0.766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.304 0.656 0.600 0.369 0.769</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.228 0.667 0.519 0.292 0.628 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.863 0.769 0.816 0.860 0.953 </t>
+  </si>
+  <si>
     <t xml:space="preserve">0.366 0.736 0.708 0.595 0.778</t>
   </si>
   <si>
@@ -198,6 +210,18 @@
     <t xml:space="preserve">0.212 0.635 0.230 0.120 0.512 </t>
   </si>
   <si>
+    <t xml:space="preserve">0.273 0.762 0.547 0.348 0.712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.471 0.623 0.715 0.606 0.852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.158 0.760 0.383 0.211 0.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.892 0.763 0.829 0.892 0.954</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(2)</t>
   </si>
   <si>
@@ -328,6 +352,75 @@
   </si>
   <si>
     <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords + Lemm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(3) + POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.415 0.728 0.636 0.466 0.727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.322 0.648 0.594 0.402 0.667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.266 0.657 0.490 0.310 0.580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.863 0.763 0.812 0.866 0.940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.337 0.711 0.642 0.466 0.728 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.363 0.529 0.530 0.406 0.698</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.205 0.825 0.508 0.310 0.580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.878 0.693 0.791 0.867 0.943 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.412 0.738 0.636 0.560 0.709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.405 0.641 0.583 0.422 0.732 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.263 0.681 0.492 0.401 0.556 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.881 0.763 0.809 0.867 0.945 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.298 0.668 0.397 0.229 0.645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.206 0.543 0.496 0.291 0.825</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.178 0.610 0.252 0.130 0.478</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.841 0.694 0.777 0.862 0.947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.249 0.766 0.560 0.366 0.710</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.463 0.619 0.734 0.598 0.752</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.143 0.778 0.396 0.225 0.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.892 0.762 0.834 0.892 0.947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(2) + POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1) + POS</t>
   </si>
   <si>
     <t xml:space="preserve">0.616 0.522 0.308 0.316 0.475</t>
@@ -992,20 +1085,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,6 +1344,18 @@
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -1259,16 +1365,16 @@
         <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1279,16 +1385,16 @@
         <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,7 +1411,7 @@
         <v>24</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>26</v>
@@ -1318,6 +1424,18 @@
       <c r="B19" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C19" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
@@ -1328,19 +1446,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1348,19 +1466,19 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1368,19 +1486,19 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,19 +1506,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,19 +1526,19 @@
         <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1432,7 +1550,7 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>33</v>
@@ -1452,7 +1570,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>37</v>
@@ -1472,7 +1590,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>18</v>
@@ -1492,7 +1610,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>41</v>
@@ -1512,7 +1630,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>44</v>
@@ -1536,19 +1654,19 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1556,19 +1674,19 @@
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,19 +1694,19 @@
         <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,19 +1714,19 @@
         <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,19 +1734,19 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1640,19 +1758,19 @@
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1660,19 +1778,19 @@
         <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,19 +1798,19 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1700,19 +1818,19 @@
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>93</v>
-      </c>
       <c r="D42" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,19 +1838,205 @@
         <v>27</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1751,20 +2055,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1802,16 +2107,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,16 +2127,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1842,16 +2147,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,16 +2167,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,16 +2187,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,16 +2211,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,16 +2231,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,16 +2251,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,16 +2271,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1986,16 +2291,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2010,16 +2315,16 @@
         <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>137</v>
+        <v>168</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2030,16 +2335,16 @@
         <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>140</v>
+        <v>171</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,16 +2355,16 @@
         <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,16 +2375,16 @@
         <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>148</v>
+        <v>179</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>149</v>
+        <v>180</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,16 +2395,16 @@
         <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>151</v>
+        <v>182</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>152</v>
+        <v>183</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>154</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,19 +2416,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>156</v>
+        <v>187</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>158</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,19 +2436,19 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>160</v>
+        <v>191</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2151,19 +2456,19 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,19 +2476,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>149</v>
+        <v>180</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,19 +2496,19 @@
         <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2215,19 +2520,19 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,19 +2540,19 @@
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2255,19 +2560,19 @@
         <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2275,19 +2580,19 @@
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,19 +2600,19 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,19 +2624,19 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2339,19 +2644,19 @@
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>180</v>
+        <v>211</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>181</v>
+        <v>212</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>182</v>
+        <v>213</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,19 +2664,19 @@
         <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>187</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2379,19 +2684,19 @@
         <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,19 +2704,19 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>195</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2423,19 +2728,19 @@
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,19 +2748,19 @@
         <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>180</v>
+        <v>211</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>181</v>
+        <v>212</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>182</v>
+        <v>213</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,19 +2768,19 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>187</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2483,19 +2788,19 @@
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2503,19 +2808,145 @@
         <v>27</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>195</v>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2534,20 +2965,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,16 +3017,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>196</v>
+        <v>227</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>197</v>
+        <v>228</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>198</v>
+        <v>229</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>199</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,16 +3037,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>201</v>
+        <v>232</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>203</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2625,16 +3057,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>204</v>
+        <v>235</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>205</v>
+        <v>236</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>206</v>
+        <v>237</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>207</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2645,16 +3077,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>209</v>
+        <v>240</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>210</v>
+        <v>241</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2665,16 +3097,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>212</v>
+        <v>243</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2689,16 +3121,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>217</v>
+        <v>248</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,16 +3141,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>223</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2729,16 +3161,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>204</v>
+        <v>235</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>205</v>
+        <v>236</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>206</v>
+        <v>237</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>207</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2749,16 +3181,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>209</v>
+        <v>240</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>210</v>
+        <v>241</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2769,16 +3201,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>226</v>
+        <v>257</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>227</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2793,16 +3225,16 @@
         <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>228</v>
+        <v>259</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>229</v>
+        <v>260</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>231</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2813,16 +3245,16 @@
         <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>232</v>
+        <v>263</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>233</v>
+        <v>264</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>234</v>
+        <v>265</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>235</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2833,16 +3265,16 @@
         <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>237</v>
+        <v>268</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>238</v>
+        <v>269</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>239</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2853,16 +3285,16 @@
         <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>241</v>
+        <v>272</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>242</v>
+        <v>273</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>243</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2873,16 +3305,16 @@
         <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>244</v>
+        <v>275</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>245</v>
+        <v>276</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>246</v>
+        <v>277</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>247</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2894,19 +3326,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>248</v>
+        <v>279</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>249</v>
+        <v>280</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2914,19 +3346,19 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>252</v>
+        <v>283</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>253</v>
+        <v>284</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>255</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2934,19 +3366,19 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>256</v>
+        <v>287</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>259</v>
+        <v>290</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2954,19 +3386,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>260</v>
+        <v>291</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>261</v>
+        <v>292</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>262</v>
+        <v>293</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>263</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2974,19 +3406,19 @@
         <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>264</v>
+        <v>295</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>265</v>
+        <v>296</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>267</v>
+        <v>298</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2998,19 +3430,19 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>217</v>
+        <v>248</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3018,19 +3450,19 @@
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>269</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3038,19 +3470,19 @@
         <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>204</v>
+        <v>235</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>205</v>
+        <v>236</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>206</v>
+        <v>237</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>207</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,19 +3490,19 @@
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>209</v>
+        <v>240</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>210</v>
+        <v>241</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3078,19 +3510,19 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>226</v>
+        <v>257</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>227</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3105,19 +3537,19 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>270</v>
+        <v>301</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>271</v>
+        <v>302</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>273</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3125,19 +3557,19 @@
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>274</v>
+        <v>305</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>276</v>
+        <v>307</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>277</v>
+        <v>308</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3145,19 +3577,19 @@
         <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>278</v>
+        <v>309</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>279</v>
+        <v>310</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>280</v>
+        <v>311</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>281</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3165,19 +3597,19 @@
         <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>282</v>
+        <v>313</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>284</v>
+        <v>315</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>285</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3185,19 +3617,19 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>286</v>
+        <v>317</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>289</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3209,19 +3641,19 @@
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>270</v>
+        <v>301</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>271</v>
+        <v>302</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>273</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3229,19 +3661,19 @@
         <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>274</v>
+        <v>305</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>276</v>
+        <v>307</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>277</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3249,19 +3681,19 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>278</v>
+        <v>309</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>279</v>
+        <v>310</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>280</v>
+        <v>311</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>281</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3269,19 +3701,19 @@
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>282</v>
+        <v>313</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>284</v>
+        <v>315</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>285</v>
+        <v>316</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3289,19 +3721,145 @@
         <v>27</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>286</v>
+        <v>317</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>289</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated keyword extraction script for IRC messages for Lucene, Thunderbird and Ubuntu
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
+++ b/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="341">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -418,6 +418,66 @@
   </si>
   <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(2) + POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.381 0.724 0.637 0.437 0.722 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.298 0.646 0.606 0.373 0.647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.239 0.649 0.490 0.285 0.575 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.860 0.761 0.816 0.861 0.937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.420 0.750 0.670 0.519 0.746</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.370 0.585 0.534 0.430 0.702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.270 0.792 0.547 0.359 0.604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.874 0.739 0.794 0.870 0.945 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.448 0.750 0.643 0.559 0.709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.406 0.657 0.560 0.456 0.732 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.293 0.694 0.505 0.398 0.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.880 0.774 0.802 0.875 0.945 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.287 0.671 0.385 0.229 0.641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.204 0.539 0.491 0.287 0.852 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.170 0.623 0.243 0.130 0.473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.842 0.692 0.776 0.861 0.948 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.243 0.762 0.571 0.367 0.707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.456 0.617 0.718 0.660 0.781</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.139 0.769 0.407 0.225 0.551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.891 0.760 0.833 0.897 0.949 </t>
   </si>
   <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1) + POS</t>
@@ -1088,7 +1148,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1963,6 +2023,18 @@
       <c r="B51" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C51" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -1971,6 +2043,18 @@
       <c r="B52" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C52" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -1979,6 +2063,18 @@
       <c r="B53" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C53" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
@@ -1987,6 +2083,18 @@
       <c r="B54" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C54" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
@@ -1995,6 +2103,18 @@
       <c r="B55" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C55" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="1"/>
@@ -2004,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,7 +2132,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2020,7 +2140,7 @@
         <v>17</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,7 +2148,7 @@
         <v>22</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2036,7 +2156,7 @@
         <v>27</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2107,16 +2227,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2127,16 +2247,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2147,16 +2267,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2167,16 +2287,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2187,16 +2307,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,16 +2331,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,16 +2351,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2251,16 +2371,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2271,16 +2391,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2291,16 +2411,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2315,16 +2435,16 @@
         <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2335,16 +2455,16 @@
         <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,16 +2475,16 @@
         <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2375,16 +2495,16 @@
         <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2395,16 +2515,16 @@
         <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2419,16 +2539,16 @@
         <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2439,16 +2559,16 @@
         <v>66</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2459,16 +2579,16 @@
         <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2479,16 +2599,16 @@
         <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,16 +2619,16 @@
         <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2523,16 +2643,16 @@
         <v>87</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2543,16 +2663,16 @@
         <v>87</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,16 +2683,16 @@
         <v>87</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,16 +2703,16 @@
         <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,16 +2723,16 @@
         <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,16 +2747,16 @@
         <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2647,16 +2767,16 @@
         <v>88</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2667,16 +2787,16 @@
         <v>88</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2687,16 +2807,16 @@
         <v>88</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2707,16 +2827,16 @@
         <v>88</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2731,16 +2851,16 @@
         <v>109</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2751,16 +2871,16 @@
         <v>109</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2771,16 +2891,16 @@
         <v>109</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2791,16 +2911,16 @@
         <v>109</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2811,16 +2931,16 @@
         <v>109</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2914,7 +3034,7 @@
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2922,7 +3042,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2930,7 +3050,7 @@
         <v>17</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,7 +3058,7 @@
         <v>22</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2946,7 +3066,7 @@
         <v>27</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3017,16 +3137,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3037,16 +3157,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3057,16 +3177,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3077,16 +3197,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3097,16 +3217,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3121,16 +3241,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3141,16 +3261,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3161,16 +3281,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,16 +3301,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3201,16 +3321,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,16 +3345,16 @@
         <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3245,16 +3365,16 @@
         <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3265,16 +3385,16 @@
         <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,16 +3405,16 @@
         <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3305,16 +3425,16 @@
         <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,16 +3449,16 @@
         <v>66</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3349,16 +3469,16 @@
         <v>66</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3369,16 +3489,16 @@
         <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3389,16 +3509,16 @@
         <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3409,16 +3529,16 @@
         <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3433,16 +3553,16 @@
         <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3453,16 +3573,16 @@
         <v>87</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3473,16 +3593,16 @@
         <v>87</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3493,16 +3613,16 @@
         <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3513,16 +3633,16 @@
         <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3540,16 +3660,16 @@
         <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3560,16 +3680,16 @@
         <v>88</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,16 +3700,16 @@
         <v>88</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3600,16 +3720,16 @@
         <v>88</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3620,16 +3740,16 @@
         <v>88</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3644,16 +3764,16 @@
         <v>109</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3664,16 +3784,16 @@
         <v>109</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3684,16 +3804,16 @@
         <v>109</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3704,16 +3824,16 @@
         <v>109</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3724,16 +3844,16 @@
         <v>109</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3827,7 +3947,7 @@
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3835,7 +3955,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,7 +3963,7 @@
         <v>17</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3851,7 +3971,7 @@
         <v>22</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3859,7 +3979,7 @@
         <v>27</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added results for fine grained classification Config 6 Label Powerset Lucene
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
+++ b/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="361">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -481,6 +481,66 @@
   </si>
   <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1) + POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.429 0.735 0.682 0.513 0.781</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.355 0.647 0.613 0.455 0.788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.278 0.671 0.549 0.352 0.647 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.870 0.765 0.823 0.876 0.955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.383 0.750 0.687 0.456 0.754 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.383 0.592 0.573 0.455 0.726 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.239 0.773 0.564 0.299 0.614</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.879 0.743 0.810 0.877 0.948 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.397 0.755 0.690 0.563 0.757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.359 0.662 0.609 0.473 0.809 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.251 0.703 0.560 0.401 0.614 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.873 0.778 0.823 0.879 0.955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.298 0.670 0.398 0.235 0.654 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.216 0.525 0.531 0.355 0.808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.178 0.639 0.252 0.134 0.488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.845 0.682 0.785 0.871 0.947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.244 0.763 0.555 0.329 0.709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.554 0.607 0.731 0.683 0.905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.139 0.789 0.390 0.197 0.551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.897 0.756 0.833 0.896 0.957</t>
   </si>
   <si>
     <t xml:space="preserve">0.616 0.522 0.308 0.316 0.475</t>
@@ -1147,8 +1207,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C63" activeCellId="0" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2126,6 +2186,18 @@
       <c r="B57" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C57" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
@@ -2134,6 +2206,18 @@
       <c r="B58" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C58" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -2142,6 +2226,18 @@
       <c r="B59" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C59" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -2150,6 +2246,18 @@
       <c r="B60" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C60" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
@@ -2157,6 +2265,18 @@
       </c>
       <c r="B61" s="1" t="s">
         <v>152</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2227,16 +2347,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2247,16 +2367,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,16 +2387,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,16 +2407,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2307,16 +2427,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2331,16 +2451,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2351,16 +2471,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,16 +2491,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2391,16 +2511,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2411,16 +2531,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2435,16 +2555,16 @@
         <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2455,16 +2575,16 @@
         <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,16 +2595,16 @@
         <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,16 +2615,16 @@
         <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2515,16 +2635,16 @@
         <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,16 +2659,16 @@
         <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2559,16 +2679,16 @@
         <v>66</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,16 +2699,16 @@
         <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2599,16 +2719,16 @@
         <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,16 +2739,16 @@
         <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2643,16 +2763,16 @@
         <v>87</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2663,16 +2783,16 @@
         <v>87</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2683,16 +2803,16 @@
         <v>87</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2703,16 +2823,16 @@
         <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2723,16 +2843,16 @@
         <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,16 +2867,16 @@
         <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2767,16 +2887,16 @@
         <v>88</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2787,16 +2907,16 @@
         <v>88</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2807,16 +2927,16 @@
         <v>88</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2827,16 +2947,16 @@
         <v>88</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2851,16 +2971,16 @@
         <v>109</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2871,16 +2991,16 @@
         <v>109</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2891,16 +3011,16 @@
         <v>109</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2911,16 +3031,16 @@
         <v>109</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2931,16 +3051,16 @@
         <v>109</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3137,16 +3257,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3157,16 +3277,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3177,16 +3297,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,16 +3317,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3217,16 +3337,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3241,16 +3361,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,16 +3381,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3281,16 +3401,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3301,16 +3421,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,16 +3441,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3345,16 +3465,16 @@
         <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,16 +3485,16 @@
         <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3385,16 +3505,16 @@
         <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3405,16 +3525,16 @@
         <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3425,16 +3545,16 @@
         <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3449,16 +3569,16 @@
         <v>66</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3469,16 +3589,16 @@
         <v>66</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3489,16 +3609,16 @@
         <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3509,16 +3629,16 @@
         <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3529,16 +3649,16 @@
         <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3553,16 +3673,16 @@
         <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3573,16 +3693,16 @@
         <v>87</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3593,16 +3713,16 @@
         <v>87</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3613,16 +3733,16 @@
         <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3633,16 +3753,16 @@
         <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3660,16 +3780,16 @@
         <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3680,16 +3800,16 @@
         <v>88</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>327</v>
+        <v>347</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3700,16 +3820,16 @@
         <v>88</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>329</v>
+        <v>349</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3720,16 +3840,16 @@
         <v>88</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3740,16 +3860,16 @@
         <v>88</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3764,16 +3884,16 @@
         <v>109</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,16 +3904,16 @@
         <v>109</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>327</v>
+        <v>347</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3804,16 +3924,16 @@
         <v>109</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>329</v>
+        <v>349</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3824,16 +3944,16 @@
         <v>109</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3844,16 +3964,16 @@
         <v>109</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added results for fine grained classification Config 6 Label Powerset Thunderbird
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
+++ b/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="421">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -823,6 +823,186 @@
   </si>
   <si>
     <t xml:space="preserve">0.774 0.865 0.927 0.933 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.602 0.469 0.302 0.310 0.446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.523 0.508 0.360 0.356 0.535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.462 0.312 0.179 0.184 0.288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.768 0.845 0.917 0.915 0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.685 0.590 0.256 0.412 0.460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.440 0.458 0.264 0.300 0.369</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.636 0.438 0.147 0.263 0.300 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.716 0.831 0.908 0.900 0.969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.568 0.643 0.390 0.481 0.489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.542 0.503 0.259 0.417 0.473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.418 0.498 0.246 0.320 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.773 0.844 0.894 0.917 0.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.389 0.258 0.044 0.060 0.399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.389 0.453 0.106 0.226 0.513 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.250 0.149 0.022 0.031 0.250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.723 0.838 0.915 0.921 0.974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.477 0.259 0.179 0.305 0.416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.588 0.900 0.846 0.820 0.955 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.321 0.149 0.098 0.180 0.263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.781 0.864 0.933 0.936 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.593 0.478 0.269 0.376 0.504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.527 0.500 0.304 0.449 0.614</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.450 0.320 0.156 0.232 0.338 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.769 0.843 0.913 0.922 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.679 0.605 0.282 0.434 0.460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.477 0.487 0.303 0.339 0.414 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.594 0.452 0.165 0.281 0.300 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.744 0.839 0.912 0.906 0.971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.595 0.641 0.395 0.460 0.475</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.555 0.493 0.263 0.385 0.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.448 0.496 0.250 0.303 0.313</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.779 0.841 0.895 0.913 0.976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.402 0.245 0.044 0.060 0.400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.405 0.456 0.125 0.280 0.556 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.261 0.140 0.022 0.031 0.250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.728 0.839 0.918 0.923 0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.470 0.271 0.201 0.279 0.431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.580 0.905 0.806 0.902 1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.315 0.157 0.112 0.162 0.275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.779 0.865 0.934 0.937 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.598 0.462 0.256 0.322 0.490 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.524 0.517 0.277 0.324 0.722 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.456 0.306 0.147 0.193 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.768 0.846 0.910 0.911 0.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.676 0.530 0.200 0.322 0.367 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.490 0.516 0.316 0.423 0.643 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.581 0.370 0.112 0.193 0.225 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.752 0.847 0.918 0.921 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.609 0.627 0.373 0.481 0.490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.566 0.490 0.268 0.424 0.703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.463 0.479 0.232 0.320 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.784 0.840 0.898 0.918 0.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.375 0.223 0.035 0.051 0.367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.396 0.445 0.114 0.162 0.621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.238 0.126 0.018 0.026 0.225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.727 0.838 0.919 0.918 0.976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.448 0.281 0.215 0.279 0.431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.642 0.940 0.871 0.925 1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.293 0.163 0.121 0.162 0.275 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.789 0.867 0.935 0.937 0.981</t>
   </si>
   <si>
     <t xml:space="preserve">0.682 0.568 0.409 0.415 0.766</t>
@@ -1207,19 +1387,19 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C63" activeCellId="0" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,19 +2477,19 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3070,6 +3250,18 @@
       <c r="B45" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C45" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
@@ -3078,6 +3270,18 @@
       <c r="B46" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C46" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
@@ -3086,6 +3290,18 @@
       <c r="B47" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C47" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -3094,6 +3310,18 @@
       <c r="B48" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C48" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
@@ -3102,6 +3330,18 @@
       <c r="B49" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C49" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="1"/>
@@ -3113,6 +3353,18 @@
       <c r="B51" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C51" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -3121,6 +3373,18 @@
       <c r="B52" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C52" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -3129,6 +3393,18 @@
       <c r="B53" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C53" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
@@ -3137,6 +3413,18 @@
       <c r="B54" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C54" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
@@ -3145,6 +3433,18 @@
       <c r="B55" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C55" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="1"/>
@@ -3156,6 +3456,18 @@
       <c r="B57" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C57" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
@@ -3164,6 +3476,18 @@
       <c r="B58" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C58" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -3172,6 +3496,18 @@
       <c r="B59" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C59" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -3180,6 +3516,18 @@
       <c r="B60" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C60" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
@@ -3187,6 +3535,18 @@
       </c>
       <c r="B61" s="1" t="s">
         <v>152</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -3213,13 +3573,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3257,16 +3617,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>267</v>
+        <v>327</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>268</v>
+        <v>328</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>269</v>
+        <v>329</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>270</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3277,16 +3637,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>271</v>
+        <v>331</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>272</v>
+        <v>332</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>273</v>
+        <v>333</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>274</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3297,16 +3657,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>275</v>
+        <v>335</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>276</v>
+        <v>336</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>278</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3317,16 +3677,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>279</v>
+        <v>339</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>280</v>
+        <v>340</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>281</v>
+        <v>341</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>282</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3337,16 +3697,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>283</v>
+        <v>343</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>284</v>
+        <v>344</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>285</v>
+        <v>345</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>286</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3361,16 +3721,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>287</v>
+        <v>347</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>288</v>
+        <v>348</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>289</v>
+        <v>349</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>290</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3381,16 +3741,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>291</v>
+        <v>351</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>292</v>
+        <v>352</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>293</v>
+        <v>353</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>294</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3401,16 +3761,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>275</v>
+        <v>335</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>276</v>
+        <v>336</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>278</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3421,16 +3781,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>279</v>
+        <v>339</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>280</v>
+        <v>340</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>281</v>
+        <v>341</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>282</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3441,16 +3801,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>295</v>
+        <v>355</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>296</v>
+        <v>356</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3465,16 +3825,16 @@
         <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>302</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3485,16 +3845,16 @@
         <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>303</v>
+        <v>363</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>304</v>
+        <v>364</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>305</v>
+        <v>365</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>306</v>
+        <v>366</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3505,16 +3865,16 @@
         <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>307</v>
+        <v>367</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>308</v>
+        <v>368</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>309</v>
+        <v>369</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>310</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3525,16 +3885,16 @@
         <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>311</v>
+        <v>371</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>312</v>
+        <v>372</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>313</v>
+        <v>373</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>314</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3545,16 +3905,16 @@
         <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>315</v>
+        <v>375</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>316</v>
+        <v>376</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>317</v>
+        <v>377</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>318</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3569,16 +3929,16 @@
         <v>66</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>319</v>
+        <v>379</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>320</v>
+        <v>380</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>321</v>
+        <v>381</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>322</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3589,16 +3949,16 @@
         <v>66</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>323</v>
+        <v>383</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>324</v>
+        <v>384</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>325</v>
+        <v>385</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>326</v>
+        <v>386</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3609,16 +3969,16 @@
         <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>327</v>
+        <v>387</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>328</v>
+        <v>388</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>329</v>
+        <v>389</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>330</v>
+        <v>390</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3629,16 +3989,16 @@
         <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>331</v>
+        <v>391</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>332</v>
+        <v>392</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>333</v>
+        <v>393</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>334</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3649,16 +4009,16 @@
         <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>335</v>
+        <v>395</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>336</v>
+        <v>396</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>337</v>
+        <v>397</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>338</v>
+        <v>398</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3673,16 +4033,16 @@
         <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>287</v>
+        <v>347</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>288</v>
+        <v>348</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>289</v>
+        <v>349</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>339</v>
+        <v>399</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3693,16 +4053,16 @@
         <v>87</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>291</v>
+        <v>351</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>292</v>
+        <v>352</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>293</v>
+        <v>353</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>340</v>
+        <v>400</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3713,16 +4073,16 @@
         <v>87</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>275</v>
+        <v>335</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>276</v>
+        <v>336</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>278</v>
+        <v>338</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3733,16 +4093,16 @@
         <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>279</v>
+        <v>339</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>280</v>
+        <v>340</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>281</v>
+        <v>341</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>282</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3753,16 +4113,16 @@
         <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>295</v>
+        <v>355</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>296</v>
+        <v>356</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3780,16 +4140,16 @@
         <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>341</v>
+        <v>401</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>342</v>
+        <v>402</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>343</v>
+        <v>403</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>344</v>
+        <v>404</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3800,16 +4160,16 @@
         <v>88</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>345</v>
+        <v>405</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>346</v>
+        <v>406</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>347</v>
+        <v>407</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>348</v>
+        <v>408</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3820,16 +4180,16 @@
         <v>88</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>349</v>
+        <v>409</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>350</v>
+        <v>410</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>351</v>
+        <v>411</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>352</v>
+        <v>412</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3840,16 +4200,16 @@
         <v>88</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>353</v>
+        <v>413</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>354</v>
+        <v>414</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>355</v>
+        <v>415</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>356</v>
+        <v>416</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3860,16 +4220,16 @@
         <v>88</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>357</v>
+        <v>417</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>358</v>
+        <v>418</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>359</v>
+        <v>419</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>360</v>
+        <v>420</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3884,16 +4244,16 @@
         <v>109</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>341</v>
+        <v>401</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>342</v>
+        <v>402</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>343</v>
+        <v>403</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>344</v>
+        <v>404</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3904,16 +4264,16 @@
         <v>109</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>345</v>
+        <v>405</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>346</v>
+        <v>406</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>347</v>
+        <v>407</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>348</v>
+        <v>408</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3924,16 +4284,16 @@
         <v>109</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>349</v>
+        <v>409</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>350</v>
+        <v>410</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>351</v>
+        <v>411</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>352</v>
+        <v>412</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3944,16 +4304,16 @@
         <v>109</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>353</v>
+        <v>413</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>354</v>
+        <v>414</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>355</v>
+        <v>415</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>356</v>
+        <v>416</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3964,16 +4324,16 @@
         <v>109</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>357</v>
+        <v>417</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>358</v>
+        <v>418</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>359</v>
+        <v>419</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>360</v>
+        <v>420</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added results for fine grained classification Config 6 Label Powerset Ubuntu
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
+++ b/thesis-fine-grained-classification/label-powerset/label-powerset-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="481">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -1285,6 +1285,186 @@
   </si>
   <si>
     <t xml:space="preserve">0.803 0.870 0.930 0.945 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.672 0.497 0.265 0.399 0.753</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.578 0.548 0.282 0.469 0.763</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.547 0.337 0.153 0.250 0.607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.790 0.861 0.916 0.944 0.976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.736 0.601 0.208 0.356 0.677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.470 0.484 0.333 0.440 0.822 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.750 0.446 0.116 0.217 0.513 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.730 0.848 0.924 0.942 0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.648 0.622 0.340 0.499 0.790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.584 0.492 0.271 0.447 0.700 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.512 0.471 0.206 0.336 0.658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.789 0.850 0.908 0.941 0.974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.492 0.205 0.062 0.039 0.713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.438 0.485 0.207 0.143 0.867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.345 0.115 0.032 0.020 0.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.729 0.852 0.926 0.940 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.639 0.356 0.191 0.282 0.755 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.619 0.881 0.952 0.781 0.947 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.495 0.217 0.106 0.164 0.607 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.800 0.880 0.939 0.952 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.671 0.522 0.369 0.407 0.759 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.584 0.519 0.368 0.433 0.735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.544 0.361 0.228 0.257 0.615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.792 0.857 0.921 0.941 0.974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.752 0.588 0.217 0.364 0.713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.501 0.494 0.354 0.442 0.867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.747 0.432 0.122 0.224 0.556 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.754 0.851 0.925 0.942 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.651 0.629 0.368 0.499 0.790 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.589 0.510 0.289 0.436 0.700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.515 0.478 0.228 0.336 0.658 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.792 0.855 0.909 0.940 0.974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.487 0.209 0.062 0.039 0.706</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.432 0.471 0.207 0.143 0.865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.341 0.117 0.032 0.020 0.547</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.726 0.850 0.926 0.940 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.644 0.353 0.191 0.282 0.761</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.635 0.854 0.952 0.758 0.947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.499 0.215 0.106 0.164 0.615 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.806 0.879 0.939 0.951 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.690 0.538 0.348 0.373 0.772 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.602 0.546 0.377 0.417 0.771</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.569 0.376 0.212 0.230 0.632 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.801 0.862 0.923 0.940 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.761 0.533 0.165 0.169 0.707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.534 0.549 0.447 0.400 0.928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.734 0.371 0.090 0.092 0.547 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.776 0.862 0.931 0.943 0.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.679 0.636 0.428 0.507 0.797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.618 0.525 0.371 0.477 0.765 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.549 0.485 0.275 0.342 0.667 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.805 0.859 0.919 0.944 0.977 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.516 0.201 0.052 0.100 0.684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.475 0.561 0.238 0.258 0.847 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.367 0.112 0.026 0.053 0.521 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.744 0.856 0.928 0.940 0.976 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.649 0.333 0.200 0.282 0.768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.676 0.854 0.955 0.833 0.948 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.501 0.200 0.111 0.164 0.624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.817 0.877 0.939 0.953 0.983</t>
   </si>
 </sst>
 </file>
@@ -2477,7 +2657,7 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
     </sheetView>
   </sheetViews>
@@ -3567,8 +3747,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4343,6 +4523,18 @@
       <c r="B45" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C45" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
@@ -4351,6 +4543,18 @@
       <c r="B46" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C46" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
@@ -4359,6 +4563,18 @@
       <c r="B47" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C47" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -4367,6 +4583,18 @@
       <c r="B48" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C48" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
@@ -4375,6 +4603,18 @@
       <c r="B49" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C49" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="1"/>
@@ -4386,6 +4626,18 @@
       <c r="B51" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C51" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -4394,6 +4646,18 @@
       <c r="B52" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C52" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -4402,6 +4666,18 @@
       <c r="B53" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C53" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
@@ -4410,6 +4686,18 @@
       <c r="B54" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C54" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
@@ -4418,6 +4706,18 @@
       <c r="B55" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C55" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="1"/>
@@ -4429,6 +4729,18 @@
       <c r="B57" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C57" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
@@ -4437,6 +4749,18 @@
       <c r="B58" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C58" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -4445,6 +4769,18 @@
       <c r="B59" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C59" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -4453,6 +4789,18 @@
       <c r="B60" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C60" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
@@ -4460,6 +4808,18 @@
       </c>
       <c r="B61" s="1" t="s">
         <v>152</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>